<commit_message>
added path related changes in preProcessor module
</commit_message>
<xml_diff>
--- a/python_code/src/preProcessor/Duplicate.xlsx
+++ b/python_code/src/preProcessor/Duplicate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,44 +455,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>794970</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>831645815</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Govardhan Reddy</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>12/6/1997</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>756415</v>
-      </c>
-      <c r="B3" t="n">
-        <v>432304732</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Swetha</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>09/30/1997</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>